<commit_message>
Until application upgrade automation nifi status check
</commit_message>
<xml_diff>
--- a/sections-blueprint.xlsx
+++ b/sections-blueprint.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/knnatarasan/hw/app/Util/cluster-automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{120363F7-43AB-1746-AF13-EBDC1C2AF574}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013A44ED-7DE3-8541-9F76-DF5E81E2D108}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16440" xr2:uid="{5AC94B5E-E414-8B46-8391-D8A05513C931}"/>
   </bookViews>
@@ -745,10 +745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DDCE952-506A-5042-8D52-29C4F1098631}">
-  <dimension ref="B2:E72"/>
+  <dimension ref="B2:F72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:E10"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -756,9 +756,10 @@
     <col min="2" max="2" width="28.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>38</v>
       </c>
@@ -768,8 +769,11 @@
       <c r="E2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>20</v>
       </c>
@@ -779,8 +783,11 @@
       <c r="E3" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -790,27 +797,27 @@
       <c r="E4" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="D5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>48</v>
       </c>
-      <c r="D6" t="s">
-        <v>35</v>
-      </c>
       <c r="E6" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>86</v>
       </c>
@@ -820,8 +827,11 @@
       <c r="E7" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>39</v>
       </c>
@@ -831,16 +841,22 @@
       <c r="E8" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D9" t="s">
         <v>11</v>
       </c>
       <c r="E9" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>80</v>
       </c>
@@ -848,7 +864,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>27</v>
       </c>
@@ -856,7 +872,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>50</v>
       </c>
@@ -867,7 +883,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>45</v>
       </c>
@@ -878,7 +894,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>109</v>
       </c>
@@ -886,7 +902,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>113</v>
       </c>
@@ -894,7 +910,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>116</v>
       </c>
@@ -984,33 +1000,21 @@
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
-        <v>4</v>
-      </c>
       <c r="D28" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
-        <v>83</v>
-      </c>
       <c r="D29" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
-        <v>54</v>
-      </c>
       <c r="D30" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
-        <v>112</v>
-      </c>
       <c r="D31" t="s">
         <v>104</v>
       </c>
@@ -1198,11 +1202,6 @@
     <row r="59" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D59" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D60" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="61" spans="4:4" x14ac:dyDescent="0.2">

</xml_diff>